<commit_message>
Helpers were created Restructured the code in cy.js files
</commit_message>
<xml_diff>
--- a/DemoTest cases.xlsx
+++ b/DemoTest cases.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\udemy certificat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079E074F-2D5D-4ADB-881A-4714F46068D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71ABA90-0E7C-4D14-A26F-1A3F83EBBCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -57,90 +54,110 @@
     <t>Test login with correct User/Pass</t>
   </si>
   <si>
-    <t>Test the login by using correct credentials.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should not be able to login </t>
-  </si>
-  <si>
     <t>Test login without credentials</t>
   </si>
   <si>
-    <t>Test the login by leaving user &amp; pass field empty</t>
-  </si>
-  <si>
-    <t>User should be able to login and taken to his
-Profile</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1.Go to https://www.demoblaze.com/</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t>Test the login by entering incorrect username/password in the username and password field</t>
+  </si>
+  <si>
+    <t>Test login with incorrect username/password</t>
+  </si>
+  <si>
+    <t>1.Go to https://www.demoblaze.com/
+2. Add correct user/pass
+3. Observe if user can login</t>
+  </si>
+  <si>
+    <t>Test the flow of an item purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if the user is able to purchase an item from the cart tab by proceeding thourgh checkout </t>
+  </si>
+  <si>
+    <t>Test adding a single item to the cart</t>
+  </si>
+  <si>
+    <t>Test the functionality of adding an item to the cart 
+and check if the item is visible in the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user should be able to place the order from the cart tab after completing the place order form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to https://www.demoblaze.com/
+2.Add incorrect username / password
+3.Observe that 
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2. Add correct user/pass
-3. Observe if user can login</t>
-    </r>
+  </si>
+  <si>
+    <t>1. Go to https://www.demoblaze.com
+2. Enter Username / Pass 
+3. Press Login
+4. Click on an item from the front page exemple "Samsung galaxy s6" then click on "Add to Cart"
+5. Click on the "Cart" button on the top of the page
+6. The item 
+7. Click on "Place Order" button 
+8. Fill out the required details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should get the following error  "Please fill out Username and Password."
+</t>
+  </si>
+  <si>
+    <t>The user should be able to add an item to the 
+cart and review it before the checkout</t>
+  </si>
+  <si>
+    <t>User: demotest123
+Password: demo12345
+Browser: Chrome</t>
+  </si>
+  <si>
+    <t>Browser: Chrome</t>
+  </si>
+  <si>
+    <t>User: demotest123*
+Password: demo12345
+Browser: Chrome</t>
   </si>
   <si>
     <t xml:space="preserve">User: demotest123
 Password: demo12345
+Browser: Chrome
 </t>
   </si>
   <si>
-    <t>User should not be able to login
-Window alert "User does not exist."</t>
-  </si>
-  <si>
-    <t>Test the login by entering incorrect username/password in the username and password field</t>
-  </si>
-  <si>
-    <t>User: dm2312
-Password: demodemo123456</t>
-  </si>
-  <si>
-    <t>Test login with incorrect username/password</t>
-  </si>
-  <si>
-    <t>1.Go to https://www.demoblaze.com/
-2.Add incorrect username/password
-3.Observe if user can login
-4. Error should pop up "User does not exist."</t>
-  </si>
-  <si>
-    <t>1.Go to http://wordpress.com
-2.Leave user &amp; login fields empty
-3.Observe if you can login
-4.Error should pop up "Please fill out Username and Password."</t>
+    <t>Test the login by leaving user / pass field empty and click on the Log-in button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to https://www.demoblaze.com
+2. Enter Username / Pass 
+3. Press Login
+4. Click on an item from the front page exemple "Samsung galaxy s6" then click on "Add to Cart"
+5. Click on the "Cart" button on the top of the page
+</t>
+  </si>
+  <si>
+    <t>1.Go to https://www.demoblaze.com
+2.Leave user / password fields empty
+3. Click Login button</t>
+  </si>
+  <si>
+    <t>User should be able to login and taken to his
+Profile page</t>
+  </si>
+  <si>
+    <t>User is informed that incorrect credentials are used and should get a window alert "User does not exist."</t>
+  </si>
+  <si>
+    <t>Test the login function entering the correct credentials in the username / pass field then press login buton.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,33 +179,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +214,11 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -211,10 +229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,19 +243,28 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -249,19 +278,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Foaie1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,23 +561,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -569,16 +585,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.25">
@@ -586,58 +602,88 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="1. Go to site.com/login_x000a_2. Add correct user/pass_x000a_3. Observe if user can login" xr:uid="{0F3D25C8-32E3-4CBF-8BE1-2D4E7A76956E}"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.demoblaze.com/" xr:uid="{638D9CA9-EE83-4408-BF3F-A35DE035DC52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>